<commit_message>
Update (things are shit)
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7044159-287C-47B8-93C2-391B76B82409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED726C-D21D-4B68-9146-671A01B1E5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>v0-17900</t>
   </si>
@@ -126,10 +126,31 @@
     <t>Relative directions</t>
   </si>
   <si>
-    <t>v45-11800</t>
-  </si>
-  <si>
     <t>Removed closest ghost direction</t>
+  </si>
+  <si>
+    <t>v5-11800</t>
+  </si>
+  <si>
+    <t>v6-8600</t>
+  </si>
+  <si>
+    <t>Fixed movement code (pacman is getting stuck now)</t>
+  </si>
+  <si>
+    <t>v7-9300</t>
+  </si>
+  <si>
+    <t>Better ghost detection, ghost distance added to reward, removed pellet reward</t>
+  </si>
+  <si>
+    <t>55 (64)</t>
+  </si>
+  <si>
+    <t>Removed learning when dying, accumulated ghost distance</t>
+  </si>
+  <si>
+    <t>v8-2500</t>
   </si>
 </sst>
 </file>
@@ -493,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,13 +915,13 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3">
         <v>77</v>
@@ -952,6 +973,192 @@
       </c>
       <c r="T7" s="1">
         <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>400</v>
+      </c>
+      <c r="J8" s="3">
+        <v>400</v>
+      </c>
+      <c r="K8" s="3">
+        <v>400</v>
+      </c>
+      <c r="L8" s="1">
+        <v>40</v>
+      </c>
+      <c r="M8" s="3">
+        <v>40</v>
+      </c>
+      <c r="N8" s="3">
+        <v>40</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>49</v>
+      </c>
+      <c r="S8" s="1">
+        <v>49</v>
+      </c>
+      <c r="T8" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1752.19</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1170</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2610</v>
+      </c>
+      <c r="L9" s="1">
+        <v>162.09</v>
+      </c>
+      <c r="M9" s="3">
+        <v>109</v>
+      </c>
+      <c r="N9" s="3">
+        <v>226</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>86.05</v>
+      </c>
+      <c r="S9" s="1">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="T9" s="1">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>110</v>
+      </c>
+      <c r="J10" s="3">
+        <v>110</v>
+      </c>
+      <c r="K10" s="3">
+        <v>110</v>
+      </c>
+      <c r="L10" s="1">
+        <v>11</v>
+      </c>
+      <c r="M10" s="3">
+        <v>11</v>
+      </c>
+      <c r="N10" s="3">
+        <v>11</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="S10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="T10" s="1">
+        <v>11.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Benchmark on new state bug fi
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1BAB1F-5C69-4C0E-8261-076913367BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F86D80-2DB3-4BF3-92F0-E8AFFBFBA892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>v0-17900</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>v9-4300</t>
+  </si>
+  <si>
+    <t>v10-3200</t>
+  </si>
+  <si>
+    <t>Fixed severe bugs in state mapping</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,6 +1235,68 @@
         <v>13.6</v>
       </c>
     </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1620</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1620</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1620</v>
+      </c>
+      <c r="L12" s="1">
+        <v>154</v>
+      </c>
+      <c r="M12" s="3">
+        <v>154</v>
+      </c>
+      <c r="N12" s="3">
+        <v>154</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>97.3</v>
+      </c>
+      <c r="S12" s="1">
+        <v>97.3</v>
+      </c>
+      <c r="T12" s="1">
+        <v>97.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V11: Fixed bug when reversing
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F86D80-2DB3-4BF3-92F0-E8AFFBFBA892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4115CE-F0D9-4830-8676-A0D368385E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>v0-17900</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Fixed severe bugs in state mapping</t>
+  </si>
+  <si>
+    <t>v11-18000</t>
+  </si>
+  <si>
+    <t>Fixed severe bug when reversing direction</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,6 +1303,68 @@
         <v>97.3</v>
       </c>
     </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3">
+        <v>85</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1838.94</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1410</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2860</v>
+      </c>
+      <c r="L13" s="1">
+        <v>171.71</v>
+      </c>
+      <c r="M13" s="3">
+        <v>133</v>
+      </c>
+      <c r="N13" s="3">
+        <v>230</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2</v>
+      </c>
+      <c r="R13" s="1">
+        <v>95.27</v>
+      </c>
+      <c r="S13" s="1">
+        <v>58.7</v>
+      </c>
+      <c r="T13" s="1">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Benchmark for V12 (pellet direction)
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4115CE-F0D9-4830-8676-A0D368385E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5636C8-2D11-452C-9D44-0695EAABB1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>v0-17900</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Fixed severe bug when reversing direction</t>
+  </si>
+  <si>
+    <t>v12-22700</t>
+  </si>
+  <si>
+    <t>Added pellet direction flag</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +550,7 @@
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="3" customWidth="1"/>
@@ -1365,6 +1371,68 @@
         <v>223</v>
       </c>
     </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>908</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1086</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2505.66</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1280</v>
+      </c>
+      <c r="K14" s="3">
+        <v>4200</v>
+      </c>
+      <c r="L14" s="1">
+        <v>221.54</v>
+      </c>
+      <c r="M14" s="3">
+        <v>114</v>
+      </c>
+      <c r="N14" s="3">
+        <v>244</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>5</v>
+      </c>
+      <c r="R14" s="1">
+        <v>132.72999999999999</v>
+      </c>
+      <c r="S14" s="1">
+        <v>58.9</v>
+      </c>
+      <c r="T14" s="1">
+        <v>308.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V16: Punishing going back
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B693F6FC-186F-4C7C-AE45-A0C4F2E6AAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785F5797-3D6E-4E95-973E-0EE349FC7A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>v0-17900</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>v15-288900</t>
+  </si>
+  <si>
+    <t>v16-4600</t>
+  </si>
+  <si>
+    <t>Punishing going back</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,6 +1643,68 @@
         <v>248</v>
       </c>
     </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>3948</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="3">
+        <v>92</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2461.96</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1270</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4130</v>
+      </c>
+      <c r="L18" s="1">
+        <v>213.89</v>
+      </c>
+      <c r="M18" s="3">
+        <v>119</v>
+      </c>
+      <c r="N18" s="3">
+        <v>244</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>4</v>
+      </c>
+      <c r="R18" s="1">
+        <v>110.75</v>
+      </c>
+      <c r="S18" s="1">
+        <v>49.7</v>
+      </c>
+      <c r="T18" s="1">
+        <v>215.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V17: Distance to pellet includes distance to node
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785F5797-3D6E-4E95-973E-0EE349FC7A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA5FE57-34B6-451E-8A25-DB07152BF475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>v0-17900</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Punishing going back</t>
+  </si>
+  <si>
+    <t>v17-700</t>
+  </si>
+  <si>
+    <t>Distance to pellet includes distance to node</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,6 +1711,68 @@
         <v>215.3</v>
       </c>
     </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <v>2749</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="3">
+        <v>58</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2588.79</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1340</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3380</v>
+      </c>
+      <c r="L19" s="1">
+        <v>229.02</v>
+      </c>
+      <c r="M19" s="3">
+        <v>130</v>
+      </c>
+      <c r="N19" s="3">
+        <v>244</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>3</v>
+      </c>
+      <c r="R19" s="1">
+        <v>100.22</v>
+      </c>
+      <c r="S19" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="T19" s="1">
+        <v>155.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Various benchmarks of V18
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA5FE57-34B6-451E-8A25-DB07152BF475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28FBA3-F5A4-47D7-A79D-E00BC24C3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>v0-17900</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>Distance to pellet includes distance to node</t>
+  </si>
+  <si>
+    <t>v17-2200</t>
+  </si>
+  <si>
+    <t>Added power pellets to state</t>
+  </si>
+  <si>
+    <t>v18-500600</t>
+  </si>
+  <si>
+    <t>v18-510800</t>
+  </si>
+  <si>
+    <t>v18-519300</t>
   </si>
 </sst>
 </file>
@@ -568,37 +583,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" style="3" customWidth="1"/>
     <col min="17" max="17" width="18" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>22</v>
       </c>
@@ -657,7 +672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -719,7 +734,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -781,7 +796,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -843,7 +858,7 @@
         <v>59.7</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -905,7 +920,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -967,7 +982,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1029,7 +1044,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1168,7 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1215,7 +1230,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1277,7 +1292,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1339,7 +1354,7 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>308.7</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1525,7 +1540,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>293.5</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1649,7 +1664,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1711,7 +1726,7 @@
         <v>215.3</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1773,7 +1788,282 @@
         <v>155.9</v>
       </c>
     </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>5325</v>
+      </c>
+      <c r="D20" s="3">
+        <v>176</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3931.59</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1630</v>
+      </c>
+      <c r="K20" s="3">
+        <v>7600</v>
+      </c>
+      <c r="L20" s="1">
+        <v>239.8</v>
+      </c>
+      <c r="M20" s="3">
+        <v>135</v>
+      </c>
+      <c r="N20" s="3">
+        <v>244</v>
+      </c>
+      <c r="O20" s="1">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>9</v>
+      </c>
+      <c r="R20" s="1">
+        <v>113.44</v>
+      </c>
+      <c r="S20" s="1">
+        <v>56.3</v>
+      </c>
+      <c r="T20" s="1">
+        <v>194.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>11395</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3">
+        <v>394</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3159.39</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1880</v>
+      </c>
+      <c r="K21" s="3">
+        <v>5450</v>
+      </c>
+      <c r="L21" s="1">
+        <v>235.48</v>
+      </c>
+      <c r="M21" s="3">
+        <v>174</v>
+      </c>
+      <c r="N21" s="3">
+        <v>244</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>7</v>
+      </c>
+      <c r="R21" s="1">
+        <v>118.17</v>
+      </c>
+      <c r="S21" s="1">
+        <v>59</v>
+      </c>
+      <c r="T21" s="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>11415</v>
+      </c>
+      <c r="D22" s="3">
+        <v>385</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.76</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>5</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4225.66</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2340</v>
+      </c>
+      <c r="K22" s="3">
+        <v>9800</v>
+      </c>
+      <c r="L22" s="1">
+        <v>239.92</v>
+      </c>
+      <c r="M22" s="3">
+        <v>164</v>
+      </c>
+      <c r="N22" s="3">
+        <v>244</v>
+      </c>
+      <c r="O22" s="1">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="P22" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>12</v>
+      </c>
+      <c r="R22" s="1">
+        <v>123.52</v>
+      </c>
+      <c r="S22" s="1">
+        <v>59.1</v>
+      </c>
+      <c r="T22" s="1">
+        <v>245.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>11422</v>
+      </c>
+      <c r="D23" s="3">
+        <v>188</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2.39</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3980.32</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2800</v>
+      </c>
+      <c r="K23" s="3">
+        <v>7400</v>
+      </c>
+      <c r="L23" s="1">
+        <v>242.65</v>
+      </c>
+      <c r="M23" s="3">
+        <v>218</v>
+      </c>
+      <c r="N23" s="3">
+        <v>244</v>
+      </c>
+      <c r="O23" s="1">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="P23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>9</v>
+      </c>
+      <c r="R23" s="1">
+        <v>101.71</v>
+      </c>
+      <c r="S23" s="1">
+        <v>64.5</v>
+      </c>
+      <c r="T23" s="1">
+        <v>207.8</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1786,7 +2076,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V19: Killing ghosts give no reward
</commit_message>
<xml_diff>
--- a/benchmark-analysis.xlsx
+++ b/benchmark-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malte\projects\pac-man-ai-reinforcement-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28FBA3-F5A4-47D7-A79D-E00BC24C3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB2940B-BF78-4D03-A5B8-82CD485FCCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20B0A376-A4EB-417F-8171-2479374C1D76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>v0-17900</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>v18-519300</t>
+  </si>
+  <si>
+    <t>v19-18300</t>
+  </si>
+  <si>
+    <t>Not including ghosts in reward</t>
   </si>
 </sst>
 </file>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6F513C-FE4A-4B60-AB2C-6BF482A293C0}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2025,6 +2031,68 @@
       </c>
       <c r="T23" s="1">
         <v>207.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <v>8071</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3">
+        <v>166</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.78</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>5</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3061.81</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2000</v>
+      </c>
+      <c r="K24" s="3">
+        <v>6400</v>
+      </c>
+      <c r="L24" s="1">
+        <v>238.52</v>
+      </c>
+      <c r="M24" s="3">
+        <v>192</v>
+      </c>
+      <c r="N24" s="3">
+        <v>244</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>7</v>
+      </c>
+      <c r="R24" s="1">
+        <v>107.5</v>
+      </c>
+      <c r="S24" s="1">
+        <v>71.3</v>
+      </c>
+      <c r="T24" s="1">
+        <v>188.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>